<commit_message>
added to the prompt that each tool from sequential agent should only run once (it was looping in tools before)
</commit_message>
<xml_diff>
--- a/pipeline_review_agent/datatesting.xlsx
+++ b/pipeline_review_agent/datatesting.xlsx
@@ -934,7 +934,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Relationship Building</t>
         </is>
       </c>
       <c r="O6" s="2" t="n">
@@ -955,13 +955,17 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>Thank You</t>
+          <t>Cultivation</t>
         </is>
       </c>
       <c r="T6" s="2" t="n">
-        <v>45889</v>
-      </c>
-      <c r="U6" t="inlineStr"/>
+        <v>45879</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Jeff Mcmullen</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">

</xml_diff>

<commit_message>
Updated the system of accessing the user's dataset in the root agent so it holds and passes the info better. also changed model back.
</commit_message>
<xml_diff>
--- a/pipeline_review_agent/datatesting.xlsx
+++ b/pipeline_review_agent/datatesting.xlsx
@@ -555,7 +555,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Tracie Jackson</t>
+          <t>John Smith</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -563,8 +563,16 @@
           <t>2024 - 25 Immune Gene Mutation Research Project</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Scholarship</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Stewardship</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>Tracie Jackson</t>
@@ -636,7 +644,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Tracie Jackson</t>
+          <t>John Smith</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -649,7 +657,11 @@
           <t>Capital Campaign</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Solicitation</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>Tracie Jackson</t>
@@ -721,7 +733,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Tracie Jackson</t>
+          <t>John Smith</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -802,7 +814,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Tracie Jackson</t>
+          <t>John Smith</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">

</xml_diff>